<commit_message>
wip: rev in workout grader
</commit_message>
<xml_diff>
--- a/src/lib/WorkoutGradeData.xlsx
+++ b/src/lib/WorkoutGradeData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dgdosen/dev/project_b_ux/src/lib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320C56F5-7F56-B347-A16E-AF63A5BB93E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443AEE1B-D1CA-1540-BA0C-19AD0599FFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="3800" windowWidth="28040" windowHeight="17440" xr2:uid="{7FDF0D22-B072-7B4B-9009-04F793CB8321}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="25100" xr2:uid="{7FDF0D22-B072-7B4B-9009-04F793CB8321}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,10 +42,10 @@
     <t>grade</t>
   </si>
   <si>
-    <t>speed</t>
+    <t>distanceFurlong</t>
   </si>
   <si>
-    <t>distanceFurlong</t>
+    <t>fps</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -410,13 +410,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -424,452 +424,452 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <f>+A2*660</f>
-        <v>660</v>
+        <v>3960</v>
       </c>
       <c r="C2">
-        <v>55</v>
+        <v>56.8</v>
       </c>
       <c r="D2">
-        <v>60</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B31" si="0">+A3*660</f>
-        <v>660</v>
+        <f>+A3*660</f>
+        <v>3960</v>
       </c>
       <c r="C3">
-        <v>56</v>
+        <v>55.8</v>
       </c>
       <c r="D3">
-        <v>70</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
-        <v>660</v>
+        <f>+A4*660</f>
+        <v>3960</v>
       </c>
       <c r="C4">
-        <v>57</v>
+        <v>54.8</v>
       </c>
       <c r="D4">
-        <v>80</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>660</v>
+        <f>+A5*660</f>
+        <v>3960</v>
       </c>
       <c r="C5">
-        <v>58</v>
+        <v>53.8</v>
       </c>
       <c r="D5">
-        <v>90</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>660</v>
+        <f>+A6*660</f>
+        <v>3960</v>
       </c>
       <c r="C6">
-        <v>59</v>
+        <v>52.8</v>
       </c>
       <c r="D6">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
-        <v>1320</v>
+        <f>+A7*660</f>
+        <v>3300</v>
       </c>
       <c r="C7">
-        <v>54.5</v>
+        <v>57</v>
       </c>
       <c r="D7">
-        <v>60</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>1320</v>
+        <f>+A8*660</f>
+        <v>3300</v>
       </c>
       <c r="C8">
-        <v>55.5</v>
+        <v>56</v>
       </c>
       <c r="D8">
-        <v>70</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>1320</v>
+        <f>+A9*660</f>
+        <v>3300</v>
       </c>
       <c r="C9">
-        <v>56.5</v>
+        <v>55</v>
       </c>
       <c r="D9">
-        <v>80</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>1320</v>
+        <f>+A10*660</f>
+        <v>3300</v>
       </c>
       <c r="C10">
-        <v>57.5</v>
+        <v>54</v>
       </c>
       <c r="D10">
-        <v>90</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
-        <v>1320</v>
+        <f>+A11*660</f>
+        <v>3300</v>
       </c>
       <c r="C11">
-        <v>58.5</v>
+        <v>53</v>
       </c>
       <c r="D11">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
-        <v>1980</v>
+        <f>+A12*660</f>
+        <v>2640</v>
       </c>
       <c r="C12">
-        <v>53.5</v>
+        <v>57.2</v>
       </c>
       <c r="D12">
-        <v>60</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
-        <v>1980</v>
+        <f>+A13*660</f>
+        <v>2640</v>
       </c>
       <c r="C13">
-        <v>54.5</v>
+        <v>56.2</v>
       </c>
       <c r="D13">
-        <v>70</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
-        <v>1980</v>
+        <f>+A14*660</f>
+        <v>2640</v>
       </c>
       <c r="C14">
-        <v>55.5</v>
+        <v>55.2</v>
       </c>
       <c r="D14">
-        <v>80</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
-        <v>1980</v>
+        <f>+A15*660</f>
+        <v>2640</v>
       </c>
       <c r="C15">
-        <v>56.5</v>
+        <v>54.2</v>
       </c>
       <c r="D15">
-        <v>90</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
-        <v>1980</v>
+        <f>+A16*660</f>
+        <v>2640</v>
       </c>
       <c r="C16">
-        <v>57.5</v>
+        <v>53.2</v>
       </c>
       <c r="D16">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
-        <v>2640</v>
+        <f>+A17*660</f>
+        <v>1980</v>
       </c>
       <c r="C17">
-        <v>53.2</v>
+        <v>57.5</v>
       </c>
       <c r="D17">
-        <v>60</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
-        <v>2640</v>
+        <f>+A18*660</f>
+        <v>1980</v>
       </c>
       <c r="C18">
-        <v>54.2</v>
+        <v>56.5</v>
       </c>
       <c r="D18">
-        <v>70</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
-        <v>2640</v>
+        <f>+A19*660</f>
+        <v>1980</v>
       </c>
       <c r="C19">
-        <v>55.2</v>
+        <v>55.5</v>
       </c>
       <c r="D19">
-        <v>80</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
-        <v>2640</v>
+        <f>+A20*660</f>
+        <v>1980</v>
       </c>
       <c r="C20">
-        <v>56.2</v>
+        <v>54.5</v>
       </c>
       <c r="D20">
-        <v>90</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
-        <v>2640</v>
+        <f>+A21*660</f>
+        <v>1980</v>
       </c>
       <c r="C21">
-        <v>57.2</v>
+        <v>53.5</v>
       </c>
       <c r="D21">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
-        <v>3300</v>
+        <f>+A22*660</f>
+        <v>1320</v>
       </c>
       <c r="C22">
-        <v>53</v>
+        <v>58.5</v>
       </c>
       <c r="D22">
-        <v>60</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B23">
-        <f t="shared" si="0"/>
-        <v>3300</v>
+        <f>+A23*660</f>
+        <v>1320</v>
       </c>
       <c r="C23">
-        <v>54</v>
+        <v>57.5</v>
       </c>
       <c r="D23">
-        <v>70</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B24">
-        <f t="shared" si="0"/>
-        <v>3300</v>
+        <f>+A24*660</f>
+        <v>1320</v>
       </c>
       <c r="C24">
-        <v>55</v>
+        <v>56.5</v>
       </c>
       <c r="D24">
-        <v>80</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B25">
-        <f t="shared" si="0"/>
-        <v>3300</v>
+        <f>+A25*660</f>
+        <v>1320</v>
       </c>
       <c r="C25">
-        <v>56</v>
+        <v>55.5</v>
       </c>
       <c r="D25">
-        <v>90</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B26">
-        <f t="shared" si="0"/>
-        <v>3300</v>
+        <f>+A26*660</f>
+        <v>1320</v>
       </c>
       <c r="C26">
-        <v>57</v>
+        <v>54.5</v>
       </c>
       <c r="D26">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B27">
-        <f t="shared" si="0"/>
-        <v>3960</v>
+        <f>+A27*660</f>
+        <v>660</v>
       </c>
       <c r="C27">
-        <v>52.8</v>
+        <v>59</v>
       </c>
       <c r="D27">
-        <v>60</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B28">
-        <f t="shared" si="0"/>
-        <v>3960</v>
+        <f>+A28*660</f>
+        <v>660</v>
       </c>
       <c r="C28">
-        <v>53.8</v>
+        <v>58</v>
       </c>
       <c r="D28">
-        <v>70</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B29">
-        <f t="shared" si="0"/>
-        <v>3960</v>
+        <f>+A29*660</f>
+        <v>660</v>
       </c>
       <c r="C29">
-        <v>54.8</v>
+        <v>57</v>
       </c>
       <c r="D29">
-        <v>80</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B30">
-        <f t="shared" si="0"/>
-        <v>3960</v>
+        <f>+A30*660</f>
+        <v>660</v>
       </c>
       <c r="C30">
-        <v>55.8</v>
+        <v>56</v>
       </c>
       <c r="D30">
-        <v>90</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B31">
-        <f t="shared" si="0"/>
-        <v>3960</v>
+        <f>+A31*660</f>
+        <v>660</v>
       </c>
       <c r="C31">
-        <v>56.8</v>
+        <v>55</v>
       </c>
       <c r="D31">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>